<commit_message>
create cross table summarizing the data
</commit_message>
<xml_diff>
--- a/01-fundamentals-descriptive-statistics/cross-table-scatter-plot.xlsx
+++ b/01-fundamentals-descriptive-statistics/cross-table-scatter-plot.xlsx
@@ -1,32 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iliya\Desktop\Statistics Course\Filming\Final excel\Section 2 - Descriptive statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\statistics-4-data-science-business-analysis\01-fundamentals-descriptive-statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1331B1DF-4298-46BB-96F3-86ED313469BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cross table" sheetId="3" r:id="rId1"/>
     <sheet name="Scatter plot" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Scatter plot</t>
   </si>
@@ -98,12 +107,42 @@
   </si>
   <si>
     <t>You have employment data about country X. You have been asked to prepare a cross-table showing that data.</t>
+  </si>
+  <si>
+    <t>Age Cohort</t>
+  </si>
+  <si>
+    <t>18 to 25</t>
+  </si>
+  <si>
+    <t>Employed</t>
+  </si>
+  <si>
+    <t>Unemployed</t>
+  </si>
+  <si>
+    <t>25 to 35</t>
+  </si>
+  <si>
+    <t>35 to 45</t>
+  </si>
+  <si>
+    <t>45 to 55</t>
+  </si>
+  <si>
+    <t>55 to 65</t>
+  </si>
+  <si>
+    <t>65+</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,14 +186,16 @@
     </font>
     <font>
       <sz val="9"/>
+      <color theme="4" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="4" tint="-0.499984740745262"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -189,10 +230,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -208,20 +250,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -229,9 +262,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -548,28 +586,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.77734375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="2:15" ht="12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
@@ -579,7 +619,7 @@
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="2:15" ht="12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -623,7 +663,7 @@
       </c>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="2:15" ht="12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
         <v>4</v>
       </c>
@@ -632,7 +672,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="2:15" ht="12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
         <v>5</v>
       </c>
@@ -641,19 +681,27 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="2:15" ht="12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="7"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="2:15" ht="12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="7"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="2:15" ht="12" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+    <row r="15" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B15" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="12"/>
@@ -665,11 +713,21 @@
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
     </row>
-    <row r="16" spans="2:15" ht="12" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="D16" s="16">
+        <f>100%-C16</f>
+        <v>0.4</v>
+      </c>
+      <c r="E16" s="16">
+        <f>SUM(C16:D16)</f>
+        <v>1</v>
+      </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="12"/>
@@ -682,10 +740,20 @@
       <c r="O16" s="11"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+      <c r="B17" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0.85</v>
+      </c>
+      <c r="D17" s="16">
+        <f>100%-C17</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="E17" s="16">
+        <f t="shared" ref="E17:E21" si="0">SUM(C17:D17)</f>
+        <v>1</v>
+      </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="12"/>
@@ -697,11 +765,21 @@
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
     </row>
-    <row r="18" spans="2:15" ht="12" x14ac:dyDescent="0.2">
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="16">
+        <f>100%-D18</f>
+        <v>0.95</v>
+      </c>
+      <c r="D18" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="E18" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="12"/>
@@ -714,10 +792,20 @@
       <c r="O18" s="11"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B19" s="11"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
+      <c r="B19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="16">
+        <f t="shared" ref="C19:C20" si="1">100%-D19</f>
+        <v>0.97</v>
+      </c>
+      <c r="D19" s="16">
+        <v>0.03</v>
+      </c>
+      <c r="E19" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
@@ -730,10 +818,20 @@
       <c r="O19" s="11"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B20" s="11"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="17"/>
+      <c r="B20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="16">
+        <f t="shared" si="1"/>
+        <v>0.97</v>
+      </c>
+      <c r="D20" s="16">
+        <v>0.03</v>
+      </c>
+      <c r="E20" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -746,10 +844,20 @@
       <c r="O20" s="11"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="11"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
+      <c r="B21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="16">
+        <v>1</v>
+      </c>
+      <c r="D21" s="16">
+        <f>100%-C21</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -761,11 +869,22 @@
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B22" s="11"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
+    <row r="22" spans="2:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B22" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="16">
+        <f>SUM(C16:C21)</f>
+        <v>5.34</v>
+      </c>
+      <c r="D22" s="16">
+        <f>SUM(D16:D21)</f>
+        <v>0.66000000000000014</v>
+      </c>
+      <c r="E22" s="16">
+        <f>SUM(E16:E21)</f>
+        <v>6</v>
+      </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -779,9 +898,9 @@
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="11"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="17"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -795,9 +914,9 @@
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="11"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="17"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="14"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -809,11 +928,11 @@
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
     </row>
-    <row r="25" spans="2:15" ht="12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="10"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="17"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -960,37 +1079,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:G163"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="3.21875" style="1" customWidth="1"/>
-    <col min="8" max="14" width="8.88671875" style="1"/>
-    <col min="15" max="15" width="5.5546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="3.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="1"/>
+    <col min="7" max="7" width="3.28515625" style="1" customWidth="1"/>
+    <col min="8" max="14" width="8.85546875" style="1"/>
+    <col min="15" max="15" width="5.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -998,7 +1117,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +1125,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
@@ -1014,7 +1133,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
@@ -1022,16 +1141,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="7"/>
     </row>
-    <row r="9" spans="2:5" ht="12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="2:5" ht="12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="7"/>
     </row>
-    <row r="12" spans="2:5" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
create clustered column chart
</commit_message>
<xml_diff>
--- a/01-fundamentals-descriptive-statistics/cross-table-scatter-plot.xlsx
+++ b/01-fundamentals-descriptive-statistics/cross-table-scatter-plot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\statistics-4-data-science-business-analysis\01-fundamentals-descriptive-statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1331B1DF-4298-46BB-96F3-86ED313469BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9777BC3C-7DBC-4E2D-BD94-599C0F33964D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -288,6 +288,1132 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Country X Employeement By Age</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cross table'!$C$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Employed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Cross table'!$B$16:$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>18 to 25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25 to 35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35 to 45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45 to 55</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55 to 65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65+</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cross table'!$C$16:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-962C-466A-86AC-27251C3CE888}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cross table'!$D$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unemployed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Cross table'!$B$16:$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>18 to 25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25 to 35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35 to 45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45 to 55</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55 to 65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65+</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cross table'!$D$16:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-962C-466A-86AC-27251C3CE888}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="403416744"/>
+        <c:axId val="403414776"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="403416744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="403414776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="403414776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="403416744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{521D34F1-86B6-AE47-A493-5B56A20C9AB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -590,7 +1716,7 @@
   <dimension ref="B1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1075,6 +2201,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
revise a scatter plot
</commit_message>
<xml_diff>
--- a/01-fundamentals-descriptive-statistics/cross-table-scatter-plot.xlsx
+++ b/01-fundamentals-descriptive-statistics/cross-table-scatter-plot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\statistics-4-data-science-business-analysis\01-fundamentals-descriptive-statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9777BC3C-7DBC-4E2D-BD94-599C0F33964D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC572E7B-5CB7-475A-B9EE-3B28ED9B2C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cross table" sheetId="3" r:id="rId1"/>
@@ -832,7 +832,1998 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Apple vs. Alphabet Stock Prices</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Scatter plot'!$D$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Alphabet (GOOGL)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Scatter plot'!$C$13:$C$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="104"/>
+                <c:pt idx="0">
+                  <c:v>116.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116.61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>117.91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>118.99</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>119.11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>119.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>119.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>119.04</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>119.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>119.78</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>120.08</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>119.97</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>121.88</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>121.94</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>121.95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>121.63</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>121.35</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>128.75</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>128.53</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>129.08000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>130.29</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>131.53</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>132.04</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>132.41999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>132.12</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>133.29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>135.02000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>135.51</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>135.34</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>135.72</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>136.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>137.11000000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>136.53</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>136.66</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>136.93</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>136.99</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>139.79</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>138.96</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>139.78</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>139.34</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>139.52000000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>138.68</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>139.13999999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>139.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>138.99</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>140.46</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>140.69</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>139.99</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>141.46</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>139.84</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>141.41999999999999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>140.91999999999999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>140.63999999999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>140.88</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>143.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>144.12</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>143.93</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>143.66</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>143.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>144.77000000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>144.02000000000001</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>143.66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>143.34</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>143.16999999999999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>141.63</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>141.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>141.05000000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>141.83000000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>141.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>140.68</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>142.44</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>142.27000000000001</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>143.63999999999999</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>144.53</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>143.68</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>143.79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>143.65</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>146.58000000000001</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>147.51</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>147.06</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>146.53</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>148.96</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>153.01</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>153.99</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>153.26</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>153.94999999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>156.1</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>155.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>155.47</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>150.25</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>152.54</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>153.06</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>153.99</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>153.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>153.34</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>153.87</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>153.61000000000001</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>153.66999999999999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>152.76</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>153.18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Scatter plot'!$D$13:$D$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="104"/>
+                <c:pt idx="0">
+                  <c:v>808.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>807.77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>813.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>825.21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>827.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>826.01</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>829.86</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>829.53</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>830.94</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>827.46</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>829.02</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>824.37</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>828.17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>844.43</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>849.53</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>858.45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>856.98</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>845.03</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>823.83</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>820.19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>815.24</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>818.26</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>820.13</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>821.62</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>829.23</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>829.88</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>830.06</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>834.85</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>838.96</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>840.03</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>837.32</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>842.17</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>846.55</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>849.27</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>851.36</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>851</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>847.81</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>849.67</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>844.93</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>856.75</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>849.85</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>849.08</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>847.27</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>851.15</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>853.64</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>857.84</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>861.4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>864.58</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>865.91</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>868.39</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>872.37</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>867.91</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>850.14</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>849.8</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>839.65</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>835.14</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>838.51</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>840.63</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>849.87</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>849.48</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>847.8</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>856.75</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>852.57</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>848.91</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>845.1</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>842.1</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>841.7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>839.88</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>841.46</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>840.18</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>855.13</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>853.99</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>856.51</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>860.08</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>858.95</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>878.93</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>888.84</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>889.14</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>891.44</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>924.52</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>932.82</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>937.09</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>948.45</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>954.72</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>950.28</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>958.69</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>956.71</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>954.84</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>955.89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>955.14</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>959.22</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>964.61</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>942.17</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>950.5</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>954.65</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>964.07</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>970.55</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>977.61</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>991.86</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>993.27</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>996.17</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>987.09</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>988.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-162A-4072-8E21-BFD043E7FDC9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="523400792"/>
+        <c:axId val="523401448"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="523400792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="110"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="523401448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="523401448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1050"/>
+          <c:min val="750"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="523400792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Apple vs. Bank of America stock prices</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2106666666666667"/>
+          <c:y val="3.2407407407407406E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Scatter plot'!$E$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bank of America (BAC)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Scatter plot'!$C$13:$C$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="104"/>
+                <c:pt idx="0">
+                  <c:v>116.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116.61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>117.91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>118.99</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>119.11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>119.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>119.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>119.04</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>119.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>119.78</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>120.08</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>119.97</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>121.88</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>121.94</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>121.95</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>121.63</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>121.35</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>128.75</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>128.53</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>129.08000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>130.29</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>131.53</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>132.04</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>132.41999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>132.12</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>133.29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>135.02000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>135.51</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>135.34</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>135.72</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>136.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>137.11000000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>136.53</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>136.66</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>136.93</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>136.99</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>139.79</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>138.96</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>139.78</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>139.34</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>139.52000000000001</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>138.68</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>139.13999999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>139.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>138.99</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>140.46</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>140.69</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>139.99</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>141.46</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>139.84</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>141.41999999999999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>140.91999999999999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>140.63999999999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>140.88</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>143.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>144.12</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>143.93</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>143.66</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>143.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>144.77000000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>144.02000000000001</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>143.66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>143.34</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>143.16999999999999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>141.63</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>141.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>141.05000000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>141.83000000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>141.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>140.68</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>142.44</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>142.27000000000001</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>143.63999999999999</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>144.53</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>143.68</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>143.79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>143.65</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>146.58000000000001</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>147.51</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>147.06</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>146.53</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>148.96</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>153.01</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>153.99</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>153.26</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>153.94999999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>156.1</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>155.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>155.47</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>150.25</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>152.54</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>153.06</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>153.99</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>153.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>153.34</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>153.87</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>153.61000000000001</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>153.66999999999999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>152.76</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>153.18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Scatter plot'!$E$13:$E$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="104"/>
+                <c:pt idx="0">
+                  <c:v>22.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.01</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.05</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.63</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.53</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22.64</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22.56</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.95</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23.37</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23.44</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23.36</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22.95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22.64</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22.89</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.72</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.29</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22.9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22.67</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>23.12</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>23.08</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>23.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>24.06</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>24.58</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>24.58</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24.52</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>24.78</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>24.79</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>24.58</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>24.23</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>24.57</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>24.68</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>25.23</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>25.44</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>25.25</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>25.21</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>25.26</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>25.35</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>25.31</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>25.3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>25.32</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>25.18</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>25.22</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>24.86</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>24.44</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>23.02</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>22.94</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>23.07</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>23.12</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>23.03</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>23.48</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>23.35</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>23.87</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>23.59</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>23.59</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>23.44</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>23.17</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>23.26</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>23.16</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>23.02</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>22.92</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>22.65</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>22.34</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>22.81</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>22.71</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>22.74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>23.07</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>22.71</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>23.63</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>23.98</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>23.89</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>23.65</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>23.34</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>23.61</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>23.53</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>23.77</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>23.85</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>23.74</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>23.96</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>23.98</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>24.15</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>24.07</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>24.06</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>23.99</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>22.57</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>22.74</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>23.05</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>23.04</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>23.39</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>23.36</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>23.25</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>23.24</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>22.91</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>22.41</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>22.63</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F676-4AA9-83A1-73EBB7B5557C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="523380128"/>
+        <c:axId val="523387016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="523380128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="523387016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="523387016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="523380128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1356,6 +3347,1038 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1408,6 +4431,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE37705B-A0C6-2B46-2884-C9E4851A5C9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>359835</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>78317</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>190502</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5402AC2F-C147-51AB-0CBD-9E611E920909}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1715,7 +4815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2209,7 +5309,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:G163"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3985,5 +7087,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>